<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-14.xlsx - 2026-01-14T06:31:34.354Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-14.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-14.xlsx
@@ -473,7 +473,7 @@
         <v>NEW</v>
       </c>
       <c r="I2" t="str">
-        <v>PENDING</v>
+        <v>PAID</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-14</v>
@@ -1073,10 +1073,10 @@
         <v>340</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G2">
-        <v>340</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-14.xlsx - 2026-01-14T06:31:38.467Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-14.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-14.xlsx
@@ -473,7 +473,7 @@
         <v>NEW</v>
       </c>
       <c r="I2" t="str">
-        <v>PAID</v>
+        <v>PENDING</v>
       </c>
       <c r="J2" t="str">
         <v>2026-01-14</v>
@@ -1073,10 +1073,10 @@
         <v>340</v>
       </c>
       <c r="F2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>325</v>
+        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Update SwaadSutra_Consolidated_2026-01-14.xlsx - 2026-01-14T17:08:07.370Z
</commit_message>
<xml_diff>
--- a/reports/SwaadSutra_Consolidated_2026-01-14.xlsx
+++ b/reports/SwaadSutra_Consolidated_2026-01-14.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,25 +449,25 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" t="str">
-        <v>2026-01-13 22:51</v>
+        <v>2026-01-14 17:08</v>
       </c>
       <c r="C2" t="str">
-        <v>Ketki</v>
+        <v>Mrunal</v>
       </c>
       <c r="D2" t="str">
-        <v>1608</v>
+        <v>KLV B 2108</v>
       </c>
       <c r="E2" t="str">
-        <v>3159135521</v>
+        <v>9404665203</v>
       </c>
       <c r="F2" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Wheat Chapati x40</v>
       </c>
       <c r="G2">
-        <v>15</v>
+        <v>600</v>
       </c>
       <c r="H2" t="str">
         <v>NEW</v>
@@ -476,10 +476,10 @@
         <v>PENDING</v>
       </c>
       <c r="J2" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K2" t="str">
-        <v>16:51</v>
+        <v>00:30</v>
       </c>
       <c r="L2" t="str">
         <v/>
@@ -493,25 +493,25 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="str">
-        <v>2026-01-13 22:43</v>
+        <v>2026-01-13 22:51</v>
       </c>
       <c r="C3" t="str">
-        <v>Swapnil (Phantom)</v>
+        <v>Ketki</v>
       </c>
       <c r="D3" t="str">
-        <v>420</v>
+        <v>1608</v>
       </c>
       <c r="E3" t="str">
-        <v/>
+        <v>3159135521</v>
       </c>
       <c r="F3" t="str">
-        <v>Vermicelli Kheer x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G3">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="H3" t="str">
         <v>NEW</v>
@@ -520,13 +520,13 @@
         <v>PENDING</v>
       </c>
       <c r="J3" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K3" t="str">
-        <v>16:42</v>
+        <v>16:51</v>
       </c>
       <c r="L3" t="str">
-        <v>No vermicelli in kheer please.</v>
+        <v/>
       </c>
       <c r="M3" t="str">
         <v/>
@@ -537,13 +537,13 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="str">
-        <v>2026-01-13 22:38</v>
+        <v>2026-01-13 22:43</v>
       </c>
       <c r="C4" t="str">
-        <v>Phantom</v>
+        <v>Swapnil (Phantom)</v>
       </c>
       <c r="D4" t="str">
         <v>420</v>
@@ -552,10 +552,10 @@
         <v/>
       </c>
       <c r="F4" t="str">
-        <v>Upma x1</v>
+        <v>Vermicelli Kheer x1</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H4" t="str">
         <v>NEW</v>
@@ -564,13 +564,13 @@
         <v>PENDING</v>
       </c>
       <c r="J4" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K4" t="str">
-        <v>15:38</v>
+        <v>16:42</v>
       </c>
       <c r="L4" t="str">
-        <v/>
+        <v>No vermicelli in kheer please.</v>
       </c>
       <c r="M4" t="str">
         <v/>
@@ -581,25 +581,25 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="str">
-        <v>2026-01-13 19:12</v>
+        <v>2026-01-13 22:38</v>
       </c>
       <c r="C5" t="str">
-        <v>Sagar Borse</v>
+        <v>Phantom</v>
       </c>
       <c r="D5" t="str">
-        <v>Yuu</v>
+        <v>420</v>
       </c>
       <c r="E5" t="str">
-        <v>7588930329</v>
+        <v/>
       </c>
       <c r="F5" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Upma x1</v>
       </c>
       <c r="G5">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H5" t="str">
         <v>NEW</v>
@@ -608,10 +608,10 @@
         <v>PENDING</v>
       </c>
       <c r="J5" t="str">
-        <v>2026-01-15</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K5" t="str">
-        <v>02:42</v>
+        <v>15:38</v>
       </c>
       <c r="L5" t="str">
         <v/>
@@ -625,16 +625,16 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="str">
-        <v>2026-01-13 19:05</v>
+        <v>2026-01-13 19:12</v>
       </c>
       <c r="C6" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D6" t="str">
-        <v>A1608</v>
+        <v>Yuu</v>
       </c>
       <c r="E6" t="str">
         <v>7588930329</v>
@@ -646,16 +646,16 @@
         <v>15</v>
       </c>
       <c r="H6" t="str">
-        <v>COOKING</v>
+        <v>NEW</v>
       </c>
       <c r="I6" t="str">
         <v>PENDING</v>
       </c>
       <c r="J6" t="str">
-        <v>2026-01-26</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K6" t="str">
-        <v>10:35</v>
+        <v>02:42</v>
       </c>
       <c r="L6" t="str">
         <v/>
@@ -669,37 +669,37 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="str">
-        <v>2026-01-13 18:59</v>
+        <v>2026-01-13 19:05</v>
       </c>
       <c r="C7" t="str">
         <v>Sagar Borse</v>
       </c>
       <c r="D7" t="str">
-        <v>A-1608</v>
+        <v>A1608</v>
       </c>
       <c r="E7" t="str">
         <v>7588930329</v>
       </c>
       <c r="F7" t="str">
-        <v>Jawar Bhakari x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G7">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="H7" t="str">
-        <v>NEW</v>
+        <v>COOKING</v>
       </c>
       <c r="I7" t="str">
         <v>PENDING</v>
       </c>
       <c r="J7" t="str">
-        <v>2026-01-16</v>
+        <v>2026-01-26</v>
       </c>
       <c r="K7" t="str">
-        <v>10:00</v>
+        <v>10:35</v>
       </c>
       <c r="L7" t="str">
         <v/>
@@ -713,25 +713,25 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="str">
-        <v>2026-01-13 16:54</v>
+        <v>2026-01-13 18:59</v>
       </c>
       <c r="C8" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D8" t="str">
-        <v>a14</v>
+        <v>A-1608</v>
       </c>
       <c r="E8" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F8" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Jawar Bhakari x1</v>
       </c>
       <c r="G8">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H8" t="str">
         <v>NEW</v>
@@ -740,10 +740,10 @@
         <v>PENDING</v>
       </c>
       <c r="J8" t="str">
-        <v/>
+        <v>2026-01-16</v>
       </c>
       <c r="K8" t="str">
-        <v/>
+        <v>10:00</v>
       </c>
       <c r="L8" t="str">
         <v/>
@@ -757,16 +757,16 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="str">
-        <v>2026-01-13 16:41</v>
+        <v>2026-01-13 16:54</v>
       </c>
       <c r="C9" t="str">
         <v>Pooja</v>
       </c>
       <c r="D9" t="str">
-        <v>saf</v>
+        <v>a14</v>
       </c>
       <c r="E9" t="str">
         <v>9096648553</v>
@@ -784,10 +784,10 @@
         <v>PENDING</v>
       </c>
       <c r="J9" t="str">
-        <v>2026-01-15</v>
+        <v/>
       </c>
       <c r="K9" t="str">
-        <v>10:12</v>
+        <v/>
       </c>
       <c r="L9" t="str">
         <v/>
@@ -801,25 +801,25 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="str">
-        <v>2026-01-13 16:40</v>
+        <v>2026-01-13 16:41</v>
       </c>
       <c r="C10" t="str">
-        <v>Sagar Borse</v>
+        <v>Pooja</v>
       </c>
       <c r="D10" t="str">
-        <v>A-1608</v>
+        <v>saf</v>
       </c>
       <c r="E10" t="str">
-        <v>7588930329</v>
+        <v>9096648553</v>
       </c>
       <c r="F10" t="str">
-        <v>Til Poli x1</v>
+        <v>Wheat Chapati x1</v>
       </c>
       <c r="G10">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="H10" t="str">
         <v>NEW</v>
@@ -828,10 +828,10 @@
         <v>PENDING</v>
       </c>
       <c r="J10" t="str">
-        <v>2026-01-14</v>
+        <v>2026-01-15</v>
       </c>
       <c r="K10" t="str">
-        <v>10:00</v>
+        <v>10:12</v>
       </c>
       <c r="L10" t="str">
         <v/>
@@ -845,25 +845,25 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11" t="str">
-        <v>2026-01-13 16:39</v>
+        <v>2026-01-13 16:40</v>
       </c>
       <c r="C11" t="str">
-        <v>Pooja</v>
+        <v>Sagar Borse</v>
       </c>
       <c r="D11" t="str">
-        <v>A1608</v>
+        <v>A-1608</v>
       </c>
       <c r="E11" t="str">
-        <v>9096648553</v>
+        <v>7588930329</v>
       </c>
       <c r="F11" t="str">
-        <v>Onion Pakoda (Kanda Bhaje) x1</v>
+        <v>Til Poli x1</v>
       </c>
       <c r="G11">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="H11" t="str">
         <v>NEW</v>
@@ -875,7 +875,7 @@
         <v>2026-01-14</v>
       </c>
       <c r="K11" t="str">
-        <v>22:09</v>
+        <v>10:00</v>
       </c>
       <c r="L11" t="str">
         <v/>
@@ -889,25 +889,25 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12" t="str">
-        <v>2026-01-13 11:15</v>
+        <v>2026-01-13 16:39</v>
       </c>
       <c r="C12" t="str">
-        <v>Ajay Dwarkunde</v>
+        <v>Pooja</v>
       </c>
       <c r="D12" t="str">
-        <v>b-703</v>
+        <v>A1608</v>
       </c>
       <c r="E12" t="str">
-        <v>8087172173</v>
+        <v>9096648553</v>
       </c>
       <c r="F12" t="str">
-        <v>Pohe x1</v>
+        <v>Onion Pakoda (Kanda Bhaje) x1</v>
       </c>
       <c r="G12">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="H12" t="str">
         <v>NEW</v>
@@ -916,10 +916,10 @@
         <v>PENDING</v>
       </c>
       <c r="J12" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="K12" t="str">
-        <v>18:50</v>
+        <v>22:09</v>
       </c>
       <c r="L12" t="str">
         <v/>
@@ -933,25 +933,25 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" t="str">
-        <v>2026-01-13 10:20</v>
+        <v>2026-01-13 11:15</v>
       </c>
       <c r="C13" t="str">
-        <v>Pooja</v>
+        <v>Ajay Dwarkunde</v>
       </c>
       <c r="D13" t="str">
-        <v>A 1608</v>
+        <v>b-703</v>
       </c>
       <c r="E13" t="str">
-        <v/>
+        <v>8087172173</v>
       </c>
       <c r="F13" t="str">
-        <v>Wheat Chapati x1</v>
+        <v>Pohe x1</v>
       </c>
       <c r="G13">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="H13" t="str">
         <v>NEW</v>
@@ -963,7 +963,7 @@
         <v>2026-01-13</v>
       </c>
       <c r="K13" t="str">
-        <v>15:50</v>
+        <v>18:50</v>
       </c>
       <c r="L13" t="str">
         <v/>
@@ -977,58 +977,102 @@
     </row>
     <row r="14">
       <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="str">
+        <v>2026-01-13 10:20</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Pooja</v>
+      </c>
+      <c r="D14" t="str">
+        <v>A 1608</v>
+      </c>
+      <c r="E14" t="str">
+        <v/>
+      </c>
+      <c r="F14" t="str">
+        <v>Wheat Chapati x1</v>
+      </c>
+      <c r="G14">
+        <v>15</v>
+      </c>
+      <c r="H14" t="str">
+        <v>NEW</v>
+      </c>
+      <c r="I14" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J14" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="K14" t="str">
+        <v>15:50</v>
+      </c>
+      <c r="L14" t="str">
+        <v/>
+      </c>
+      <c r="M14" t="str">
+        <v/>
+      </c>
+      <c r="N14" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
         <v>1</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B15" t="str">
         <v>2026-01-13 10:09</v>
       </c>
-      <c r="C14" t="str">
+      <c r="C15" t="str">
         <v>Anuradha N</v>
       </c>
-      <c r="D14" t="str">
+      <c r="D15" t="str">
         <v>B 304</v>
       </c>
-      <c r="E14" t="str">
-        <v/>
-      </c>
-      <c r="F14" t="str">
+      <c r="E15" t="str">
+        <v/>
+      </c>
+      <c r="F15" t="str">
         <v>Til Poli x1</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <v>30</v>
       </c>
-      <c r="H14" t="str">
+      <c r="H15" t="str">
         <v>COOKING</v>
       </c>
-      <c r="I14" t="str">
-        <v>PENDING</v>
-      </c>
-      <c r="J14" t="str">
+      <c r="I15" t="str">
+        <v>PENDING</v>
+      </c>
+      <c r="J15" t="str">
         <v>2026-01-14</v>
       </c>
-      <c r="K14" t="str">
+      <c r="K15" t="str">
         <v>16:45</v>
       </c>
-      <c r="L14" t="str">
-        <v/>
-      </c>
-      <c r="M14" t="str">
-        <v/>
-      </c>
-      <c r="N14" t="str">
+      <c r="L15" t="str">
+        <v/>
+      </c>
+      <c r="M15" t="str">
+        <v/>
+      </c>
+      <c r="N15" t="str">
         <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N15"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1058,10 +1102,10 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2026-01-13</v>
+        <v>2026-01-14</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1070,18 +1114,41 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>340</v>
+        <v>600</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>2026-01-13</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>340</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
         <v>340</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>